<commit_message>
making progress understanding files
</commit_message>
<xml_diff>
--- a/doc/gradrho_files.xlsx
+++ b/doc/gradrho_files.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlw\Documents\Research\ORIGFORKS\mpi-sppy\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlw\Documents\Research\NOTDLW\mpi-sppy\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E680E2-B2A5-43D4-AA6C-3655E53BD7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070944FA-2C99-4D4A-869F-2516AAC5C191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3792" yWindow="732" windowWidth="17280" windowHeight="5316" xr2:uid="{B7F98E89-4BD3-46E6-8C56-AF72331F22AB}"/>
+    <workbookView xWindow="1545" yWindow="90" windowWidth="34140" windowHeight="20295" xr2:uid="{B7F98E89-4BD3-46E6-8C56-AF72331F22AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>mpi-sppy gradrho files</t>
   </si>
@@ -65,40 +65,96 @@
     <t>grad_rho_file</t>
   </si>
   <si>
-    <t>what_path</t>
-  </si>
-  <si>
     <t>rho_file</t>
   </si>
   <si>
     <t>rho_path</t>
   </si>
   <si>
-    <t>extensions.gradient_extension.py; utils.gradient.py</t>
-  </si>
-  <si>
     <t>utils.find_rho.py; utils.gradient.py</t>
   </si>
   <si>
-    <t>see also extensions.gradient_extension.py where the name is cached then the cfg is overwritten with a temp file (and not a good temp file)</t>
-  </si>
-  <si>
     <t>(findstr /s xxxx *.py)</t>
   </si>
   <si>
-    <t xml:space="preserve">cylinders.ph_ob.py; gradient_extension.py; utils.find_rho.py; </t>
-  </si>
-  <si>
     <t>cylinders.ph_ob.py; gradient_extension.py; utils.find_rho.py; utils.gradient.py</t>
+  </si>
+  <si>
+    <t>extensions.gradient_extension.py; utils.gradient.py; in ph_ob.py it is overwritten with a bad temp file name (but the file is deleted later)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">see also extensions.gradient_extension.py where the name is cached then the cfg is overwritten with a temp file (and not a good temp file), ditto in </t>
+  </si>
+  <si>
+    <t>utils.gradient.py</t>
+  </si>
+  <si>
+    <t>assigned to whatpath in find_grad_rho (currently in grandient.py)</t>
+  </si>
+  <si>
+    <t>whatpath</t>
+  </si>
+  <si>
+    <t>utils.find_rho.py</t>
+  </si>
+  <si>
+    <t>the Find_Rho class requires this file; the values are assigned to self.c</t>
+  </si>
+  <si>
+    <t>grad_cost_file == '' causes find_grad_rho to do nothing</t>
+  </si>
+  <si>
+    <t>They are treated as costs for the rho formula, so they are not really a W-hat, I think</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>the Find_Rho class needs either rho_file or a grad_rho file</t>
+  </si>
+  <si>
+    <t>See compute_rho in find_rho.py</t>
+  </si>
+  <si>
+    <t>NOT USED</t>
+  </si>
+  <si>
+    <t>rho_file is no longer used</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>rho_setter (where it is aka rhofile)</t>
+  </si>
+  <si>
+    <t>cylinders.ph_ob.py; gradient_extension.py; utils.find_rho.py;  used in a good-old-fashioned rho_setter function (it might be written as grad_rho_file)</t>
+  </si>
+  <si>
+    <t>Grad_cost_file gets read as whatpath</t>
+  </si>
+  <si>
+    <t>grad_rho_file gets read as rho_path</t>
+  </si>
+  <si>
+    <t>These names should be udpated…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -125,9 +181,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,19 +519,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C8E953C-3376-425D-9958-E858114FD2A4}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="28.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" customWidth="1"/>
+    <col min="5" max="5" width="63.7109375" customWidth="1"/>
+    <col min="6" max="6" width="66.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -482,70 +542,141 @@
         <v>45444</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>7</v>
       </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
       <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" t="s">
         <v>13</v>
       </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>10</v>
       </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="s">
-        <v>16</v>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[WIP] changing to cost_file_in and cost_file_out in the cfg
</commit_message>
<xml_diff>
--- a/doc/gradrho_files.xlsx
+++ b/doc/gradrho_files.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t xml:space="preserve">mpi-sppy gradrho files</t>
   </si>
@@ -103,6 +103,9 @@
     <t xml:space="preserve">cylinders.ph_ob.py; gradient_extension.py; utils.find_rho.py;  used in a good-old-fashioned rho_setter function (it might be written as grad_rho_file)</t>
   </si>
   <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
     <t xml:space="preserve">Notes:</t>
   </si>
   <si>
@@ -124,7 +127,10 @@
     <t xml:space="preserve">These names should be udpated…</t>
   </si>
   <si>
-    <t xml:space="preserve">plan</t>
+    <t xml:space="preserve">Plan:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nearly</t>
   </si>
   <si>
     <t xml:space="preserve">whatpath becomes grad_cost_file_in</t>
@@ -133,6 +139,9 @@
     <t xml:space="preserve">grad_cost_file becomes grad_cost_file_out</t>
   </si>
   <si>
+    <t xml:space="preserve">TBD from JPW-  why are these two here at all? SHOULD NOT BE IN THE "GRADIENT" FILE</t>
+  </si>
+  <si>
     <t xml:space="preserve">rho_path becomes rho_file_in</t>
   </si>
   <si>
@@ -143,6 +152,12 @@
   </si>
   <si>
     <t xml:space="preserve">! There will not be a use_grad_cost: grad_cost_in or compute_grad_cost implies it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deal with writing grad_cost_file_out to a temp file in gradient_extension.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        print("\n Calling find_grad_costs; note that it will not write them\n")</t>
   </si>
 </sst>
 </file>
@@ -257,10 +272,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -382,74 +397,104 @@
         <v>26</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>36</v>
+      </c>
       <c r="B33" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
[WIP] working on cfg and functions that do what they are called
</commit_message>
<xml_diff>
--- a/doc/gradrho_files.xlsx
+++ b/doc/gradrho_files.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t xml:space="preserve">mpi-sppy gradrho files</t>
   </si>
@@ -158,6 +158,21 @@
   </si>
   <si>
     <t xml:space="preserve">        print("\n Calling find_grad_costs; note that it will not write them\n")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">look at ph_ob file use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find_Rho should be able to use W’s (see get_rho_from_W)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">look into find_grad_rho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fix grad_cost_and_rho (see also the test)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">farmer_rho_demo.bash</t>
   </si>
 </sst>
 </file>
@@ -272,10 +287,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -464,11 +479,17 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>36</v>
+      </c>
       <c r="B35" s="0" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>36</v>
+      </c>
       <c r="B36" s="0" t="s">
         <v>41</v>
       </c>
@@ -495,6 +516,31 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
only one test fails, but it is the most important: test_grad_extensions
</commit_message>
<xml_diff>
--- a/doc/gradrho_files.xlsx
+++ b/doc/gradrho_files.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t xml:space="preserve">mpi-sppy gradrho files</t>
   </si>
@@ -173,6 +173,18 @@
   </si>
   <si>
     <t xml:space="preserve">farmer_rho_demo.bash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grad_cost_and_rho vs. Find_Rho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grad_cost_and_rho writes files; Find_Rho reads them</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grad_extension.mid_iter: are things computed before being written?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The test py file needs better file setup and cleanup (e.g., get rid of _out files)</t>
   </si>
 </sst>
 </file>
@@ -287,10 +299,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
+      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -541,6 +553,24 @@
         <v>50</v>
       </c>
     </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>